<commit_message>
version con distribuciones buenas
</commit_message>
<xml_diff>
--- a/jumbo/Datos_jumbo.xlsx
+++ b/jumbo/Datos_jumbo.xlsx
@@ -1171,700 +1171,700 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>00:04:16</t>
+          <t>00:02:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>00:04:44</t>
+          <t>00:03:09</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>00:01:34</t>
+          <t>00:01:03</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>00:08:38</t>
+          <t>00:05:45</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:00:34</t>
+          <t>00:00:22</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00:08:34</t>
+          <t>00:05:42</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>00:01:52</t>
+          <t>00:01:15</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>00:04:19</t>
+          <t>00:02:52</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>00:04:11</t>
+          <t>00:02:47</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>00:11:55</t>
+          <t>00:07:56</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>00:10:52</t>
+          <t>00:07:14</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>00:00:07</t>
+          <t>00:00:04</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:01</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>00:02:21</t>
+          <t>00:01:34</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:04</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>00:03:12</t>
+          <t>00:02:08</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>00:02:17</t>
+          <t>00:01:31</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>00:03:17</t>
+          <t>00:02:11</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>00:01:44</t>
+          <t>00:01:09</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>00:00:57</t>
+          <t>00:00:38</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>00:08:58</t>
+          <t>00:05:58</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>00:03:54</t>
+          <t>00:02:36</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>00:00:18</t>
+          <t>00:00:12</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>00:02:59</t>
+          <t>00:01:59</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>00:01:01</t>
+          <t>00:00:40</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>00:01:34</t>
+          <t>00:01:02</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>00:04:33</t>
+          <t>00:03:02</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>00:01:18</t>
+          <t>00:00:52</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>00:07:48</t>
+          <t>00:05:12</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>00:03:49</t>
+          <t>00:02:32</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>00:02:24</t>
+          <t>00:01:36</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>00:00:35</t>
+          <t>00:00:23</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>00:01:34</t>
+          <t>00:01:03</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>00:04:19</t>
+          <t>00:02:52</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>00:14:03</t>
+          <t>00:09:22</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>00:00:13</t>
+          <t>00:00:09</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>00:00:26</t>
+          <t>00:00:17</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>00:04:02</t>
+          <t>00:02:41</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>00:05:23</t>
+          <t>00:03:35</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:00:11</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>00:05:18</t>
+          <t>00:03:32</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>00:04:38</t>
+          <t>00:03:05</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>00:03:29</t>
+          <t>00:02:19</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>00:01:14</t>
+          <t>00:00:49</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>00:01:45</t>
+          <t>00:01:10</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>00:01:22</t>
+          <t>00:00:54</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>00:05:30</t>
+          <t>00:03:40</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>00:01:11</t>
+          <t>00:00:47</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>00:01:10</t>
+          <t>00:00:46</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>00:08:12</t>
+          <t>00:05:28</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>00:07:34</t>
+          <t>00:05:03</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>00:10:23</t>
+          <t>00:06:55</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>00:04:56</t>
+          <t>00:03:17</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:00:10</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>00:00:17</t>
+          <t>00:00:11</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>00:02:26</t>
+          <t>00:01:37</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>00:05:49</t>
+          <t>00:03:52</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>00:06:28</t>
+          <t>00:04:18</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>00:03:02</t>
+          <t>00:02:01</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>00:09:21</t>
+          <t>00:06:14</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>00:00:29</t>
+          <t>00:00:19</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>00:00:45</t>
+          <t>00:00:30</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>00:01:12</t>
+          <t>00:00:48</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>00:00:53</t>
+          <t>00:00:35</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>00:01:07</t>
+          <t>00:00:44</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:15</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>00:01:24</t>
+          <t>00:00:56</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:03</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>00:02:18</t>
+          <t>00:01:32</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>00:08:44</t>
+          <t>00:05:49</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>00:01:46</t>
+          <t>00:01:10</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>00:02:56</t>
+          <t>00:01:57</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>00:02:50</t>
+          <t>00:01:53</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>00:08:07</t>
+          <t>00:05:25</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>00:03:58</t>
+          <t>00:02:39</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>00:05:13</t>
+          <t>00:03:29</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>00:01:13</t>
+          <t>00:00:49</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>00:07:08</t>
+          <t>00:04:45</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>00:00:36</t>
+          <t>00:00:24</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>00:01:34</t>
+          <t>00:01:02</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>00:04:00</t>
+          <t>00:02:40</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>00:01:13</t>
+          <t>00:00:48</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>00:06:31</t>
+          <t>00:04:20</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>00:05:54</t>
+          <t>00:03:56</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:00:21</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>00:00:47</t>
+          <t>00:00:31</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>00:00:09</t>
+          <t>00:00:06</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>00:05:52</t>
+          <t>00:03:54</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>00:01:14</t>
+          <t>00:00:49</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>00:01:29</t>
+          <t>00:00:59</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>00:00:56</t>
+          <t>00:00:37</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>00:00:23</t>
+          <t>00:00:15</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>00:01:49</t>
+          <t>00:01:13</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>00:00:48</t>
+          <t>00:00:32</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>00:02:29</t>
+          <t>00:01:39</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>00:00:40</t>
+          <t>00:00:27</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>00:02:08</t>
+          <t>00:01:25</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>00:08:53</t>
+          <t>00:05:55</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>00:01:23</t>
+          <t>00:00:55</t>
         </is>
       </c>
     </row>

</xml_diff>